<commit_message>
baseURL changed navbar menu created
</commit_message>
<xml_diff>
--- a/public/resources/statistics.xlsx
+++ b/public/resources/statistics.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\zsebtanar3\public\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\zsebtanar4\public\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10344" windowHeight="2904"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="7404"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -19,33 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Classes</t>
-  </si>
-  <si>
-    <t>Topics</t>
-  </si>
-  <si>
-    <t>Subtopics</t>
-  </si>
-  <si>
-    <t>Definitions</t>
-  </si>
-  <si>
-    <t>Quiz</t>
-  </si>
-  <si>
     <t>Exercises</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>2015.11.07</t>
   </si>
 </sst>
 </file>
@@ -397,71 +376,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="6" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
typeahead search (in progress...)
</commit_message>
<xml_diff>
--- a/public/resources/statistics.xlsx
+++ b/public/resources/statistics.xlsx
@@ -1,44 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\zsebtanar4\public\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="7404"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>Exercises</t>
   </si>
+  <si>
+    <t>2015.11.21</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -49,43 +56,34 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="none"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -375,19 +373,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,9 +396,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
check exercises READY :)
</commit_message>
<xml_diff>
--- a/public/resources/statistics.xlsx
+++ b/public/resources/statistics.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>2015.11.21</t>
+  </si>
+  <si>
+    <t>2015.11.25</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -402,6 +405,14 @@
       </c>
       <c r="B2">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exercise links DONE :)
</commit_message>
<xml_diff>
--- a/public/resources/statistics.xlsx
+++ b/public/resources/statistics.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>2015.11.25</t>
+  </si>
+  <si>
+    <t>2015.11.26</t>
   </si>
 </sst>
 </file>
@@ -380,7 +383,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A2" sqref="A2"/>
@@ -413,6 +416,14 @@
       </c>
       <c r="B3">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>